<commit_message>
Merge main and resolve conflict in Erfstadt_v1.json
</commit_message>
<xml_diff>
--- a/BiogasDisplay/datasets/Erfstadt_v1.xlsx
+++ b/BiogasDisplay/datasets/Erfstadt_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OAtmaca\Desktop\operations-hub-widgets\BiogasDisplay\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B803521E-F831-4488-AA06-5E25CE1ADC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5B42DE-E06C-4B67-90FE-F589B8D3C412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36040" yWindow="-8820" windowWidth="21600" windowHeight="11300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26000" yWindow="-7170" windowWidth="21600" windowHeight="11300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="143">
   <si>
     <t>Variable</t>
   </si>
@@ -469,12 +469,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -484,6 +478,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -509,9 +510,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -796,677 +798,783 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="62.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="62.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="48.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E2" s="1"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="A4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="A7" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="A10" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="A11" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F12" s="1"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="A14" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="A15" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="A18" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="A19" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="A22" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="A23" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="A26" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="A27" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="A28" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="A29" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="A30" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="A31" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="A32" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+      <c r="A33" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+      <c r="A34" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="A37" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+      <c r="A38" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="A39" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+      <c r="A40" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+      <c r="A41" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+      <c r="A42" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+      <c r="A43" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+      <c r="A44" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+      <c r="A45" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+      <c r="A46" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+      <c r="A47" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
+      <c r="A50" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
+      <c r="A51" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
+      <c r="A52" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+      <c r="A53" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
+      <c r="A54" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="2" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
cluster excel file added
</commit_message>
<xml_diff>
--- a/BiogasDisplay/datasets/Erfstadt_v1.xlsx
+++ b/BiogasDisplay/datasets/Erfstadt_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OAtmaca\Desktop\operations-hub-widgets\BiogasDisplay\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5B42DE-E06C-4B67-90FE-F589B8D3C412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D952E7-2261-4ABD-9E21-D3B6DFE36A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26000" yWindow="-7170" windowWidth="21600" windowHeight="11300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="147">
   <si>
     <t>Variable</t>
   </si>
@@ -454,6 +454,18 @@
   </si>
   <si>
     <t>Title</t>
+  </si>
+  <si>
+    <t>Timeline</t>
+  </si>
+  <si>
+    <t>Cluster</t>
+  </si>
+  <si>
+    <t>Anlage</t>
+  </si>
+  <si>
+    <t>Erftstadt</t>
   </si>
 </sst>
 </file>
@@ -510,10 +522,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -795,782 +806,1065 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="62.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="62.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="48.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" t="s">
         <v>133</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" t="s">
         <v>121</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" t="s">
         <v>133</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" t="s">
         <v>134</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="D6" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="E6" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="F6" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" t="s">
         <v>134</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="D7" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="F7" t="s">
         <v>80</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" t="s">
         <v>135</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="D9" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="E9" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="F9" t="s">
         <v>118</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="G9" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" t="s">
         <v>135</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="D10" t="s">
         <v>119</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="E10" t="s">
         <v>120</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="G10" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" t="s">
         <v>135</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="D11" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="E11" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="F11" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="G11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>146</v>
+      </c>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" t="s">
         <v>136</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="D13" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="E13" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="F13" t="s">
         <v>80</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="G13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C14" t="s">
         <v>136</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="D14" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="E14" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="F14" t="s">
         <v>79</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="G14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" t="s">
         <v>136</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="D15" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="E15" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="F15" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="G15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" t="s">
         <v>137</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="D17" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="E17" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="F17" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="G17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>146</v>
+      </c>
+      <c r="C18" t="s">
         <v>137</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="D18" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="E18" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="F18" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="G18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>146</v>
+      </c>
+      <c r="C19" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="D19" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="E19" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="F19" t="s">
         <v>79</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="G19" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C21" t="s">
         <v>138</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="D21" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="E21" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="F21" t="s">
         <v>80</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="G21" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" t="s">
         <v>138</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="D22" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="E22" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="F22" t="s">
         <v>79</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="G22" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>146</v>
+      </c>
+      <c r="C23" t="s">
         <v>138</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="D23" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="E23" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="F23" t="s">
         <v>79</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="G23" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C25" t="s">
         <v>139</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="D25" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="E25" t="s">
         <v>124</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="F25" t="s">
         <v>78</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="G25" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>146</v>
+      </c>
+      <c r="C26" t="s">
         <v>139</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="D26" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="E26" t="s">
         <v>125</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="F26" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="G26" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" t="s">
         <v>139</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="D27" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="E27" t="s">
         <v>126</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="F27" t="s">
         <v>78</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="G27" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="H27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>146</v>
+      </c>
+      <c r="C28" t="s">
         <v>139</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="D28" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="E28" t="s">
         <v>127</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="F28" t="s">
         <v>77</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="G28" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>146</v>
+      </c>
+      <c r="C29" t="s">
         <v>139</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="D29" t="s">
         <v>83</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="E29" t="s">
         <v>128</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="F29" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="G29" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="H29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>146</v>
+      </c>
+      <c r="C30" t="s">
         <v>139</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="D30" t="s">
         <v>83</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="E30" t="s">
         <v>129</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="F30" t="s">
         <v>77</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="G30" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>146</v>
+      </c>
+      <c r="C31" t="s">
         <v>139</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="D31" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="E31" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="F31" t="s">
         <v>78</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="G31" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" t="s">
         <v>139</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="D32" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="E32" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="F32" t="s">
         <v>77</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="G32" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>146</v>
+      </c>
+      <c r="C33" t="s">
         <v>139</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="D33" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="E33" t="s">
         <v>130</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="F33" t="s">
         <v>77</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="G33" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="H33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>146</v>
+      </c>
+      <c r="C34" t="s">
         <v>139</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="D34" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="E34" t="s">
         <v>131</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="F34" t="s">
         <v>78</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="G34" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>146</v>
+      </c>
+      <c r="C36" t="s">
         <v>140</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="D36" t="s">
         <v>89</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="E36" t="s">
         <v>90</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="F36" t="s">
         <v>80</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="G36" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="H36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>146</v>
+      </c>
+      <c r="C37" t="s">
         <v>140</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="D37" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="E37" t="s">
         <v>92</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="F37" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="G37" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="H37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>146</v>
+      </c>
+      <c r="C38" t="s">
         <v>140</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="D38" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="E38" t="s">
         <v>94</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="F38" t="s">
         <v>80</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="G38" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="H38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>146</v>
+      </c>
+      <c r="C39" t="s">
         <v>140</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="D39" t="s">
         <v>95</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="E39" t="s">
         <v>96</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="F39" t="s">
         <v>79</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="G39" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="H39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>146</v>
+      </c>
+      <c r="C40" t="s">
         <v>140</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="D40" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="E40" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="F40" t="s">
         <v>80</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="G40" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="H40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" t="s">
         <v>140</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="D41" t="s">
         <v>99</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="E41" t="s">
         <v>100</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="F41" t="s">
         <v>79</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="G41" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="H41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>146</v>
+      </c>
+      <c r="C42" t="s">
         <v>140</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="D42" t="s">
         <v>101</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="E42" t="s">
         <v>102</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="F42" t="s">
         <v>80</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="G42" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="H42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>146</v>
+      </c>
+      <c r="C43" t="s">
         <v>140</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="D43" t="s">
         <v>103</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="E43" t="s">
         <v>104</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="F43" t="s">
         <v>79</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="G43" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="H43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>146</v>
+      </c>
+      <c r="C44" t="s">
         <v>140</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="D44" t="s">
         <v>105</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="E44" t="s">
         <v>106</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="F44" t="s">
         <v>80</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="G44" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="H44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>146</v>
+      </c>
+      <c r="C45" t="s">
         <v>140</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="D45" t="s">
         <v>107</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="E45" t="s">
         <v>108</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="F45" t="s">
         <v>79</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="G45" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="H45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46" t="s">
         <v>140</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="D46" t="s">
         <v>109</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="E46" t="s">
         <v>110</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="F46" t="s">
         <v>80</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="G46" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="H46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>146</v>
+      </c>
+      <c r="C47" t="s">
         <v>140</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="D47" t="s">
         <v>111</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="E47" t="s">
         <v>112</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="F47" t="s">
         <v>79</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="G47" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="H47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>146</v>
+      </c>
+      <c r="C49" t="s">
         <v>141</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="E49" t="s">
         <v>113</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="F49" t="s">
         <v>2</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="G49" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="H49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" t="s">
         <v>141</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="E50" t="s">
         <v>114</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="F50" t="s">
         <v>2</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="G50" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="H50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>146</v>
+      </c>
+      <c r="C51" t="s">
         <v>141</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="E51" t="s">
         <v>115</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="F51" t="s">
         <v>2</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="G51" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="H51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>146</v>
+      </c>
+      <c r="C52" t="s">
         <v>141</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="E52" t="s">
         <v>116</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="F52" t="s">
         <v>2</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="G52" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="H52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>146</v>
+      </c>
+      <c r="C53" t="s">
         <v>141</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="D53" t="s">
         <v>74</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="E53" t="s">
         <v>75</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="F53" t="s">
         <v>76</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="G53" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+      <c r="H53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>146</v>
+      </c>
+      <c r="C54" t="s">
         <v>141</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="E54" t="s">
         <v>117</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="F54" t="s">
         <v>76</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="G54" t="s">
         <v>44</v>
+      </c>
+      <c r="H54" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>